<commit_message>
implemented Student question ask to tutor answered functionality with additional API of Question Timing with dynamic Timing for all questions
</commit_message>
<xml_diff>
--- a/new_details.xlsx
+++ b/new_details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t xml:space="preserve">when question go to re answer it goes to same tiutor then we senfd the que to admin so he can give anwer </t>
   </si>
@@ -173,6 +173,9 @@
       </rPr>
       <t>. In their wallet and in case of deletation of account he can reddem it.</t>
     </r>
+  </si>
+  <si>
+    <t>For new Question  refer to note</t>
   </si>
 </sst>
 </file>
@@ -598,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1021,7 +1024,9 @@
       <c r="A109" s="1"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="1"/>
+      <c r="A110" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>

</xml_diff>